<commit_message>
Cleaned data in exampledata2. Made scatterplot and boxplot with new 'exploratory' variables with eda data. New figures can be found in /results/figures.
</commit_message>
<xml_diff>
--- a/data/raw-data/exampledata2.xlsx
+++ b/data/raw-data/exampledata2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10118"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C0CD150-280E-F24C-9BAF-08408040BF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7498B6FA-1B14-4942-BB26-C56CF0880C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Height</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>L/G/R/O/NA</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -419,7 +428,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -451,6 +460,12 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -462,6 +477,12 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -473,6 +494,12 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -484,6 +511,12 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
+      <c r="D5">
+        <v>7.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -495,6 +528,12 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -506,6 +545,12 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
+      <c r="D7">
+        <v>5.5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -517,6 +562,12 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -528,6 +579,12 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -539,6 +596,12 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
+      <c r="D10">
+        <v>5.5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -550,6 +613,12 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -558,6 +627,12 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -569,6 +644,12 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
+      <c r="D13">
+        <v>4.5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -580,6 +661,12 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
+      <c r="D14">
+        <v>5.5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -590,6 +677,12 @@
       </c>
       <c r="C15" t="s">
         <v>3</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding actual data to what was due on Tuesday
</commit_message>
<xml_diff>
--- a/data/raw-data/exampledata2.xlsx
+++ b/data/raw-data/exampledata2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C0CD150-280E-F24C-9BAF-08408040BF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3E8A807-6EBF-744A-ABF3-039A80D91F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Height</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>L/G/R/O/NA</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -419,7 +428,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -451,6 +460,12 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -462,6 +477,12 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -473,6 +494,12 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -484,6 +511,12 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
+      <c r="D5">
+        <v>7.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -495,6 +528,12 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -506,6 +545,12 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
+      <c r="D7">
+        <v>5.5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -517,6 +562,12 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -528,6 +579,12 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -539,6 +596,12 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
+      <c r="D10">
+        <v>5.5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -550,6 +613,12 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -558,6 +627,12 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -569,6 +644,12 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
+      <c r="D13">
+        <v>4.5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -580,6 +661,12 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
+      <c r="D14">
+        <v>5.5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -590,6 +677,12 @@
       </c>
       <c r="C15" t="s">
         <v>3</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>